<commit_message>
feat: 添加 HTML 卡片 GIF 导出工具 (v1.1.1)
- 新增 GifExportTool 组件，支持将 HTML 字符串中的卡片元素导出为动画 GIF 或静态 PNG
- 添加 GIF 导出相关的 API 处理程序和预加载脚本
- 更新主页面集成新的 GIF 导出工具
- 添加中英文翻译支持
- 更新应用版本至 1.1.1
- 更新 changelog 记录新功能
</commit_message>
<xml_diff>
--- a/resources/candidates.xlsx
+++ b/resources/candidates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="23720"/>
+    <workbookView windowWidth="24960" windowHeight="13740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <author>corry</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0">
+    <comment ref="C1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -38,11 +38,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="155">
   <si>
     <t>*姓名</t>
   </si>
   <si>
+    <t>*证件类型</t>
+  </si>
+  <si>
     <t>*身份证号</t>
   </si>
   <si>
@@ -56,6 +59,9 @@
   </si>
   <si>
     <t>齐月</t>
+  </si>
+  <si>
+    <t>居民身份证</t>
   </si>
   <si>
     <t>110228199409302615</t>
@@ -504,10 +510,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -537,13 +543,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="微软雅黑"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="等线"/>
       <charset val="134"/>
@@ -551,6 +550,13 @@
     <font>
       <sz val="10"/>
       <name val="等线"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
     <font>
@@ -576,45 +582,6 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -623,22 +590,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -654,7 +606,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -668,16 +620,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -692,7 +666,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -719,13 +725,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -737,43 +881,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -785,121 +905,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -952,17 +958,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -993,30 +993,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1040,150 +1016,180 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1206,16 +1212,16 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1746,18 +1752,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M108" sqref="M108"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelCol="5"/>
   <cols>
-    <col min="5" max="5" width="13.8461538461538"/>
+    <col min="6" max="6" width="13.8461538461538"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="35.25" customHeight="1" spans="1:5">
+    <row r="1" s="1" customFormat="1" ht="35.25" customHeight="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1767,843 +1773,993 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" s="1" customFormat="1" ht="48.95" customHeight="1" spans="1:5">
-      <c r="A2" s="6" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+    </row>
+    <row r="2" s="1" customFormat="1" ht="48.95" customHeight="1" spans="1:6">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6">
+      <c r="D2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5">
         <v>18311022386</v>
       </c>
     </row>
-    <row r="3" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="6" t="s">
+    <row r="3" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="6">
+      <c r="B3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5">
         <v>13000000007</v>
       </c>
     </row>
-    <row r="4" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="6" t="s">
+    <row r="4" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="6">
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5">
         <v>15260000829</v>
       </c>
     </row>
-    <row r="5" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="6" t="s">
+    <row r="5" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="6">
+      <c r="B5" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="5">
         <v>18600000462</v>
       </c>
     </row>
-    <row r="6" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="6" t="s">
+    <row r="6" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="6">
+      <c r="B6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="5">
         <v>15310000190</v>
       </c>
     </row>
-    <row r="7" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="6" t="s">
+    <row r="7" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="6">
+      <c r="B7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="5">
         <v>18600000836</v>
       </c>
     </row>
-    <row r="8" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="6" t="s">
+    <row r="8" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="6">
+      <c r="B8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="5">
         <v>18100000220</v>
       </c>
     </row>
-    <row r="9" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="6" t="s">
+    <row r="9" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A9" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="6">
+      <c r="B9" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="5">
         <v>17600000631</v>
       </c>
     </row>
-    <row r="10" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="6" t="s">
+    <row r="10" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="6">
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="5">
         <v>18810000277</v>
       </c>
     </row>
-    <row r="11" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="9" t="s">
+    <row r="11" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="6">
+      <c r="B11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="5">
         <v>18010000489</v>
       </c>
     </row>
-    <row r="12" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="6" t="s">
+    <row r="12" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="6">
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="5">
         <v>18810000794</v>
       </c>
     </row>
-    <row r="13" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A13" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="6" t="s">
+    <row r="13" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="6">
+      <c r="B13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="5">
         <v>15110000067</v>
       </c>
     </row>
-    <row r="14" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A14" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="6" t="s">
+    <row r="14" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="6">
+      <c r="B14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="5">
         <v>18800000654</v>
       </c>
     </row>
-    <row r="15" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="6" t="s">
+    <row r="15" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A15" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="6">
+      <c r="B15" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="5">
         <v>18800000652</v>
       </c>
     </row>
-    <row r="16" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A16" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="6" t="s">
+    <row r="16" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="6">
+      <c r="B16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" s="5">
         <v>13650000811</v>
       </c>
     </row>
-    <row r="17" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A17" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="9" t="s">
+    <row r="17" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A17" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="6">
+      <c r="B17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="5">
         <v>18240000021</v>
       </c>
     </row>
-    <row r="18" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A18" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="6" t="s">
+    <row r="18" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A18" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="6">
+      <c r="B18" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="5">
         <v>18820000157</v>
       </c>
     </row>
-    <row r="19" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A19" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="6" t="s">
+    <row r="19" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A19" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="6">
+      <c r="B19" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" s="5">
         <v>17340000770</v>
       </c>
     </row>
-    <row r="20" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A20" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="6" t="s">
+    <row r="20" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A20" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="E20" s="6">
+      <c r="B20" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" s="5">
         <v>15810000975</v>
       </c>
     </row>
-    <row r="21" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A21" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="6" t="s">
+    <row r="21" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A21" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="6">
+      <c r="B21" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" s="5">
         <v>13850000250</v>
       </c>
     </row>
-    <row r="22" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A22" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="6" t="s">
+    <row r="22" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A22" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="6">
+      <c r="B22" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="5">
         <v>18190000926</v>
       </c>
     </row>
-    <row r="23" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A23" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="6" t="s">
+    <row r="23" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E23" s="6">
+      <c r="B23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="5">
         <v>15210000732</v>
       </c>
     </row>
-    <row r="24" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:5">
-      <c r="A24" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="6" t="s">
+    <row r="24" s="2" customFormat="1" ht="24.75" customHeight="1" spans="1:6">
+      <c r="A24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E24" s="6">
+      <c r="B24" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="5">
         <v>18810000300</v>
       </c>
     </row>
-    <row r="25" s="2" customFormat="1" spans="1:5">
-      <c r="A25" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="6" t="s">
+    <row r="25" s="2" customFormat="1" spans="1:6">
+      <c r="A25" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="E25" s="6">
+      <c r="B25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="5">
         <v>19800000702</v>
       </c>
     </row>
-    <row r="26" s="2" customFormat="1" spans="1:5">
-      <c r="A26" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="6" t="s">
+    <row r="26" s="2" customFormat="1" spans="1:6">
+      <c r="A26" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E26" s="6">
+      <c r="B26" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" s="5">
         <v>13580000199</v>
       </c>
     </row>
-    <row r="27" s="2" customFormat="1" spans="1:5">
-      <c r="A27" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D27" s="6" t="s">
+    <row r="27" s="2" customFormat="1" spans="1:6">
+      <c r="A27" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="6">
+      <c r="B27" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="5">
         <v>15530000676</v>
       </c>
     </row>
-    <row r="28" s="2" customFormat="1" spans="1:5">
-      <c r="A28" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D28" s="6" t="s">
+    <row r="28" s="2" customFormat="1" spans="1:6">
+      <c r="A28" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E28" s="6">
+      <c r="B28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="5">
         <v>13320000915</v>
       </c>
     </row>
-    <row r="29" s="2" customFormat="1" spans="1:5">
-      <c r="A29" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="6" t="s">
+    <row r="29" s="2" customFormat="1" spans="1:6">
+      <c r="A29" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="E29" s="6">
+      <c r="B29" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" s="5">
         <v>18710000266</v>
       </c>
     </row>
-    <row r="30" s="2" customFormat="1" spans="1:5">
-      <c r="A30" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="6" t="s">
+    <row r="30" s="2" customFormat="1" spans="1:6">
+      <c r="A30" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E30" s="6">
+      <c r="B30" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" s="5">
         <v>18810000108</v>
       </c>
     </row>
-    <row r="31" s="2" customFormat="1" spans="1:5">
-      <c r="A31" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="6" t="s">
+    <row r="31" s="2" customFormat="1" spans="1:6">
+      <c r="A31" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="6">
+      <c r="B31" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F31" s="5">
         <v>17330000823</v>
       </c>
     </row>
-    <row r="32" s="3" customFormat="1" spans="1:5">
-      <c r="A32" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="6" t="s">
+    <row r="32" s="3" customFormat="1" spans="1:6">
+      <c r="A32" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E32" s="6">
+      <c r="B32" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32" s="5">
         <v>17390000837</v>
       </c>
     </row>
-    <row r="33" s="3" customFormat="1" spans="1:5">
-      <c r="A33" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D33" s="6" t="s">
+    <row r="33" s="3" customFormat="1" spans="1:6">
+      <c r="A33" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="6">
+      <c r="B33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F33" s="5">
         <v>13710000879</v>
       </c>
     </row>
-    <row r="34" s="3" customFormat="1" spans="1:5">
-      <c r="A34" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D34" s="6" t="s">
+    <row r="34" s="3" customFormat="1" spans="1:6">
+      <c r="A34" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E34" s="6">
+      <c r="B34" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F34" s="5">
         <v>18610000517</v>
       </c>
     </row>
-    <row r="35" s="3" customFormat="1" spans="1:5">
-      <c r="A35" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="6" t="s">
+    <row r="35" s="3" customFormat="1" spans="1:6">
+      <c r="A35" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E35" s="6">
+      <c r="B35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F35" s="5">
         <v>13900000868</v>
       </c>
     </row>
-    <row r="36" s="3" customFormat="1" spans="1:5">
-      <c r="A36" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="6" t="s">
+    <row r="36" s="3" customFormat="1" spans="1:6">
+      <c r="A36" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E36" s="6">
+      <c r="B36" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F36" s="5">
         <v>18810000459</v>
       </c>
     </row>
-    <row r="37" s="3" customFormat="1" spans="1:5">
-      <c r="A37" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="6" t="s">
+    <row r="37" s="3" customFormat="1" spans="1:6">
+      <c r="A37" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E37" s="6">
+      <c r="B37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" s="5">
         <v>18850000519</v>
       </c>
     </row>
-    <row r="38" s="3" customFormat="1" spans="1:5">
-      <c r="A38" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="6" t="s">
+    <row r="38" s="3" customFormat="1" spans="1:6">
+      <c r="A38" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E38" s="6">
+      <c r="B38" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" s="5">
         <v>18010000912</v>
       </c>
     </row>
-    <row r="39" s="3" customFormat="1" spans="1:5">
-      <c r="A39" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="6" t="s">
+    <row r="39" s="3" customFormat="1" spans="1:6">
+      <c r="A39" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E39" s="6">
+      <c r="B39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F39" s="5">
         <v>18810000726</v>
       </c>
     </row>
-    <row r="40" s="3" customFormat="1" spans="1:5">
-      <c r="A40" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="6" t="s">
+    <row r="40" s="3" customFormat="1" spans="1:6">
+      <c r="A40" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="E40" s="6">
+      <c r="B40" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F40" s="5">
         <v>18810000028</v>
       </c>
     </row>
-    <row r="41" s="3" customFormat="1" spans="1:5">
-      <c r="A41" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="6" t="s">
+    <row r="41" s="3" customFormat="1" spans="1:6">
+      <c r="A41" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E41" s="6">
+      <c r="B41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F41" s="5">
         <v>18810000399</v>
       </c>
     </row>
-    <row r="42" s="3" customFormat="1" spans="1:5">
-      <c r="A42" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="6" t="s">
+    <row r="42" s="3" customFormat="1" spans="1:6">
+      <c r="A42" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="E42" s="6">
+      <c r="B42" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F42" s="5">
         <v>18810000618</v>
       </c>
     </row>
-    <row r="43" s="3" customFormat="1" spans="1:5">
-      <c r="A43" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="6" t="s">
+    <row r="43" s="3" customFormat="1" spans="1:6">
+      <c r="A43" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E43" s="6">
+      <c r="B43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="F43" s="5">
         <v>15820000580</v>
       </c>
     </row>
-    <row r="44" s="3" customFormat="1" spans="1:5">
-      <c r="A44" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="6" t="s">
+    <row r="44" s="3" customFormat="1" spans="1:6">
+      <c r="A44" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E44" s="6">
+      <c r="B44" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F44" s="5">
         <v>17770000453</v>
       </c>
     </row>
-    <row r="45" s="3" customFormat="1" spans="1:5">
-      <c r="A45" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D45" s="6" t="s">
+    <row r="45" s="3" customFormat="1" spans="1:6">
+      <c r="A45" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="E45" s="6">
+      <c r="B45" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F45" s="5">
         <v>19800000905</v>
       </c>
     </row>
-    <row r="46" s="3" customFormat="1" spans="1:5">
-      <c r="A46" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D46" s="6" t="s">
+    <row r="46" s="3" customFormat="1" spans="1:6">
+      <c r="A46" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E46" s="6">
+      <c r="B46" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F46" s="5">
         <v>18810000962</v>
       </c>
     </row>
-    <row r="47" s="3" customFormat="1" spans="1:5">
-      <c r="A47" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D47" s="6" t="s">
+    <row r="47" s="3" customFormat="1" spans="1:6">
+      <c r="A47" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E47" s="6">
+      <c r="B47" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="F47" s="5">
         <v>13140000161</v>
       </c>
     </row>
-    <row r="48" s="3" customFormat="1" spans="1:5">
-      <c r="A48" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D48" s="6" t="s">
+    <row r="48" s="3" customFormat="1" spans="1:6">
+      <c r="A48" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E48" s="6">
+      <c r="B48" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F48" s="5">
         <v>18310000788</v>
       </c>
     </row>
-    <row r="49" s="3" customFormat="1" spans="1:5">
-      <c r="A49" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D49" s="6" t="s">
+    <row r="49" s="3" customFormat="1" spans="1:6">
+      <c r="A49" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E49" s="6">
+      <c r="B49" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F49" s="5">
         <v>18610000486</v>
       </c>
     </row>
-    <row r="50" s="3" customFormat="1" spans="1:5">
-      <c r="A50" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D50" s="6" t="s">
+    <row r="50" s="3" customFormat="1" spans="1:6">
+      <c r="A50" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E50" s="6">
+      <c r="B50" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F50" s="5">
         <v>19370000686</v>
       </c>
     </row>

</xml_diff>